<commit_message>
completar tratamiento de datos / agregar funciones / otros
</commit_message>
<xml_diff>
--- a/reportes_odoo/reporte.xlsx
+++ b/reportes_odoo/reporte.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
   <si>
     <t>Total</t>
   </si>
@@ -37,21 +37,27 @@
     <t xml:space="preserve">          agosto 2022</t>
   </si>
   <si>
+    <t xml:space="preserve">     [E-COM08] Caja de almacenaje</t>
+  </si>
+  <si>
     <t xml:space="preserve">     [E-COM10] Cubo de pedal</t>
   </si>
   <si>
+    <t xml:space="preserve">          junio 2022</t>
+  </si>
+  <si>
     <t xml:space="preserve">     [E-COM11] Gabinete con puertas</t>
   </si>
   <si>
     <t xml:space="preserve">     [FURN_0096] Escritorio personalizable (Acero, Blanco)</t>
   </si>
   <si>
+    <t xml:space="preserve">     [FURN_0098] Escritorio personalizable (Aluminio, Blanco)</t>
+  </si>
+  <si>
     <t xml:space="preserve">     [FURN_0269] Silla de oficina negra</t>
   </si>
   <si>
-    <t xml:space="preserve">          junio 2022</t>
-  </si>
-  <si>
     <t xml:space="preserve">     [FURN_6666] Pantallas de bloque acústico</t>
   </si>
   <si>
@@ -68,12 +74,6 @@
   </si>
   <si>
     <t xml:space="preserve">     [FURN_8999] Sofá de tres asientos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Diseño interior virtual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Área de casa virtual</t>
   </si>
 </sst>
 </file>
@@ -422,7 +422,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -448,7 +448,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="3">
-        <v>284</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -456,7 +456,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -464,7 +464,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -512,7 +512,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -520,7 +520,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -528,20 +528,20 @@
         <v>8</v>
       </c>
       <c r="B13" s="3">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B14" s="3">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B15" s="3">
         <v>1</v>
@@ -549,18 +549,18 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B16" s="3">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B17" s="3">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -568,7 +568,7 @@
         <v>11</v>
       </c>
       <c r="B18" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -576,7 +576,7 @@
         <v>3</v>
       </c>
       <c r="B19" s="3">
-        <v>23</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -584,23 +584,23 @@
         <v>12</v>
       </c>
       <c r="B20" s="3">
-        <v>53</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B21" s="3">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B22" s="3">
-        <v>43</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -608,76 +608,76 @@
         <v>13</v>
       </c>
       <c r="B23" s="3">
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B24" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B25" s="3">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B26" s="3">
-        <v>4</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B27" s="3">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B28" s="3">
-        <v>1</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B29" s="3">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B30" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B31" s="3">
-        <v>22</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B32" s="3">
         <v>11</v>
@@ -685,66 +685,82 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B33" s="3">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="B34" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B35" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B36" s="3">
-        <v>74</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B37" s="3">
-        <v>48</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B38" s="3">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B39" s="3">
-        <v>60</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="3">
         <v>11</v>
       </c>
-      <c r="B40" s="3">
-        <v>60</v>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B42" s="3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>